<commit_message>
Added Standard BlackScholes Put valuations
</commit_message>
<xml_diff>
--- a/test/data/BlackScholes.xlsx
+++ b/test/data/BlackScholes.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Spot</t>
   </si>
@@ -43,6 +46,9 @@
   </si>
   <si>
     <t>'=q_EstandarBlackScholes_old(C17,C18,C19,C20,C21,C22,C23,"Call")</t>
+  </si>
+  <si>
+    <t>Puto</t>
   </si>
 </sst>
 </file>
@@ -78,11 +84,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -97,8 +105,28 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet2"/>
+      <sheetName val="Sheet3"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="q_EstandarBlackScholes"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -387,34 +415,36 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A4:J3097"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:J698"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
     <col min="5" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>100</v>
+      <c r="C4" s="5">
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="C5">
-        <v>110</v>
+      <c r="C5" s="5">
+        <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -422,24 +452,38 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="2">
-        <f ca="1">TODAY()</f>
-        <v>41992</v>
+        <v>42003</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="4">
+        <f>C7</f>
+        <v>42003</v>
+      </c>
+      <c r="E7">
+        <v>42003</v>
+      </c>
+      <c r="F7" s="2">
+        <f>E7</f>
+        <v>42003</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="2">
         <v>42723</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="4">
+        <f>C8</f>
+        <v>42723</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -447,7 +491,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -455,21 +499,21 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" t="b">
-        <v>1</v>
+      <c r="C11" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C12">
-        <f ca="1">_xll.q_EstandarBlackScholes(C4,C5,C6,C7,C8,C9,C10,C11)</f>
-        <v>126918.33</v>
+        <f>[1]!q_EstandarBlackScholes(C4,C5,C6,C7,C8,C9,C10,C11)</f>
+        <v>0.16388842368450629</v>
       </c>
       <c r="D12">
         <v>11.086780894364313</v>
@@ -481,7 +525,7 @@
       </c>
       <c r="B17">
         <f ca="1">100+RAND()*100</f>
-        <v>106.95172461044969</v>
+        <v>170.08506541054714</v>
       </c>
       <c r="C17">
         <v>110</v>
@@ -491,7 +535,7 @@
       </c>
       <c r="E17" s="2">
         <f ca="1">TODAY()</f>
-        <v>41992</v>
+        <v>42018</v>
       </c>
       <c r="F17" s="2">
         <v>42723</v>
@@ -505,9 +549,9 @@
       <c r="I17" t="b">
         <v>1</v>
       </c>
-      <c r="J17">
-        <f ca="1">_xll.q_EstandarBlackScholes(B17,C17,D17,E17,F17,G17,H17,I17)</f>
-        <v>126925.28172461045</v>
+      <c r="J17" t="str">
+        <f>"q_EstandarBlackScholes(B17;C17;D17;E17;F17;G17;H17;I17)"</f>
+        <v>q_EstandarBlackScholes(B17;C17;D17;E17;F17;G17;H17;I17)</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -515,8 +559,8 @@
         <v>2</v>
       </c>
       <c r="B18">
-        <f t="shared" ref="B18:B81" ca="1" si="0">100+RAND()*100</f>
-        <v>167.77120010087464</v>
+        <f t="shared" ref="B18:B23" ca="1" si="0">100+RAND()*100</f>
+        <v>147.33762908785872</v>
       </c>
       <c r="C18">
         <v>110</v>
@@ -525,8 +569,8 @@
         <v>0.05</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" ref="E18:E81" ca="1" si="1">TODAY()</f>
-        <v>41992</v>
+        <f t="shared" ref="E18:E23" ca="1" si="1">TODAY()</f>
+        <v>42018</v>
       </c>
       <c r="F18" s="2">
         <v>42723</v>
@@ -540,9 +584,9 @@
       <c r="I18" t="b">
         <v>1</v>
       </c>
-      <c r="J18">
-        <f ca="1">_xll.q_EstandarBlackScholes(B18,C18,D18,E18,F18,G18,H18,I18)</f>
-        <v>126986.10120010088</v>
+      <c r="J18" t="str">
+        <f t="shared" ref="J18:J23" si="2">"q_EstandarBlackScholes(B17;C17;D17;E17;F17;G17;H17;I17)"</f>
+        <v>q_EstandarBlackScholes(B17;C17;D17;E17;F17;G17;H17;I17)</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -551,7 +595,7 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>163.25132208142276</v>
+        <v>154.64843023366728</v>
       </c>
       <c r="C19">
         <v>110</v>
@@ -561,7 +605,7 @@
       </c>
       <c r="E19" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>41992</v>
+        <v>42018</v>
       </c>
       <c r="F19" s="2">
         <v>42723</v>
@@ -575,9 +619,9 @@
       <c r="I19" t="b">
         <v>1</v>
       </c>
-      <c r="J19">
-        <f ca="1">_xll.q_EstandarBlackScholes(B19,C19,D19,E19,F19,G19,H19,I19)</f>
-        <v>126981.58132208142</v>
+      <c r="J19" t="str">
+        <f t="shared" si="2"/>
+        <v>q_EstandarBlackScholes(B17;C17;D17;E17;F17;G17;H17;I17)</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -586,7 +630,7 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>101.43069775881503</v>
+        <v>173.16696467957635</v>
       </c>
       <c r="C20">
         <v>110</v>
@@ -596,7 +640,7 @@
       </c>
       <c r="E20" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>41992</v>
+        <v>42018</v>
       </c>
       <c r="F20" s="2">
         <v>42723</v>
@@ -610,9 +654,9 @@
       <c r="I20" t="b">
         <v>1</v>
       </c>
-      <c r="J20">
-        <f ca="1">_xll.q_EstandarBlackScholes(B20,C20,D20,E20,F20,G20,H20,I20)</f>
-        <v>126919.76069775881</v>
+      <c r="J20" t="str">
+        <f t="shared" si="2"/>
+        <v>q_EstandarBlackScholes(B17;C17;D17;E17;F17;G17;H17;I17)</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -621,7 +665,7 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>172.30084929805588</v>
+        <v>125.80768668880154</v>
       </c>
       <c r="C21">
         <v>110</v>
@@ -631,7 +675,7 @@
       </c>
       <c r="E21" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>41992</v>
+        <v>42018</v>
       </c>
       <c r="F21" s="2">
         <v>42723</v>
@@ -645,9 +689,9 @@
       <c r="I21" t="b">
         <v>1</v>
       </c>
-      <c r="J21">
-        <f ca="1">_xll.q_EstandarBlackScholes(B21,C21,D21,E21,F21,G21,H21,I21)</f>
-        <v>126990.63084929806</v>
+      <c r="J21" t="str">
+        <f t="shared" si="2"/>
+        <v>q_EstandarBlackScholes(B17;C17;D17;E17;F17;G17;H17;I17)</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -656,7 +700,7 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>136.62245600507978</v>
+        <v>107.27908154539129</v>
       </c>
       <c r="C22">
         <v>110</v>
@@ -666,7 +710,7 @@
       </c>
       <c r="E22" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>41992</v>
+        <v>42018</v>
       </c>
       <c r="F22" s="2">
         <v>42723</v>
@@ -680,9 +724,9 @@
       <c r="I22" t="b">
         <v>1</v>
       </c>
-      <c r="J22">
-        <f ca="1">_xll.q_EstandarBlackScholes(B22,C22,D22,E22,F22,G22,H22,I22)</f>
-        <v>126954.95245600508</v>
+      <c r="J22" t="str">
+        <f t="shared" si="2"/>
+        <v>q_EstandarBlackScholes(B17;C17;D17;E17;F17;G17;H17;I17)</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -691,7 +735,7 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>150.06002544194419</v>
+        <v>146.7818507769891</v>
       </c>
       <c r="C23">
         <v>110</v>
@@ -701,7 +745,7 @@
       </c>
       <c r="E23" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>41992</v>
+        <v>42018</v>
       </c>
       <c r="F23" s="2">
         <v>42723</v>
@@ -715,9 +759,9 @@
       <c r="I23" t="b">
         <v>1</v>
       </c>
-      <c r="J23">
-        <f ca="1">_xll.q_EstandarBlackScholes(B23,C23,D23,E23,F23,G23,H23,I23)</f>
-        <v>126968.39002544194</v>
+      <c r="J23" t="str">
+        <f t="shared" si="2"/>
+        <v>q_EstandarBlackScholes(B17;C17;D17;E17;F17;G17;H17;I17)</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -22240,6 +22284,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -22250,7 +22295,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22263,7 +22308,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>